<commit_message>
All files regarding to project moved to Doc directoty
</commit_message>
<xml_diff>
--- a/Doc/excel gpio.xlsx
+++ b/Doc/excel gpio.xlsx
@@ -119,16 +119,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +425,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,8 +439,8 @@
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -508,13 +509,38 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="27" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G27" s="1"/>

</xml_diff>